<commit_message>
update testpoints and testoutput datasets
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_doaggregate_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_doaggregate_10pts_1miles.xlsx
@@ -2129,72 +2129,75 @@
     <t xml:space="preserve">State percentile for % Asian (non-Hispanic, single race)</t>
   </si>
   <si>
+    <t xml:space="preserve">State percentile for % American Indian and Alaska Native (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Native Hawaiian and Other Pacific Islander (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Other race (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % Two or more races (non-Hispanic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % White (non-Hispanic, single race)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for % with Disabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State percentile for %Low life expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for Demographic Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for Supplemental EJ Index for Supplemental Demographic Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % Low Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % in limited English-speaking Households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % Unemployed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % with Less Than High School Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % under Age 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % over Age 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Average for % People of Color</t>
+  </si>
+  <si>
     <t xml:space="preserve">26</t>
   </si>
   <si>
-    <t xml:space="preserve">State percentile for % American Indian and Alaska Native (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Native Hawaiian and Other Pacific Islander (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Other race (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % Two or more races (non-Hispanic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % White (non-Hispanic, single race)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for % with Disabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State percentile for %Low life expectancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for Demographic Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for Supplemental EJ Index for Supplemental Demographic Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % Low Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % in limited English-speaking Households</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % Unemployed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % with Less Than High School Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % under Age 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % over Age 64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Average for % People of Color</t>
-  </si>
-  <si>
     <t xml:space="preserve">State Average for % Hispanic or Latino</t>
   </si>
   <si>
@@ -2453,13 +2456,16 @@
     <t xml:space="preserve">State percentile for Superfund Proximity (site count/km distance)</t>
   </si>
   <si>
+    <t xml:space="preserve">82</t>
+  </si>
+  <si>
     <t xml:space="preserve">State percentile for RMP Proximity (facility count/km distance)</t>
   </si>
   <si>
     <t xml:space="preserve">State percentile for Hazardous Waste Proximity (facility count/km distance)</t>
   </si>
   <si>
-    <t xml:space="preserve">44</t>
+    <t xml:space="preserve">47</t>
   </si>
   <si>
     <t xml:space="preserve">State percentile for Underground Storage Tanks (UST) indicator</t>
@@ -2567,9 +2573,6 @@
     <t xml:space="preserve">US percentile for EJ Index for Toxic Releases to Air</t>
   </si>
   <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for EJ Index for Traffic Proximity and Volume</t>
   </si>
   <si>
@@ -2577,9 +2580,6 @@
   </si>
   <si>
     <t xml:space="preserve">US percentile for EJ Index for Lead Paint Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
   </si>
   <si>
     <t xml:space="preserve">US percentile for EJ Index for Superfund Proximity</t>
@@ -4576,10 +4576,10 @@
         <v>701</v>
       </c>
       <c r="FQ1" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="FR1" s="11" t="s">
         <v>703</v>
-      </c>
-      <c r="FR1" s="11" t="s">
-        <v>704</v>
       </c>
       <c r="FS1" s="11" t="s">
         <v>705</v>
@@ -4624,250 +4624,250 @@
         <v>723</v>
       </c>
       <c r="GG1" s="7" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="GH1" s="7" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="GI1" s="7" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="GJ1" s="7" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="GK1" s="7" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="GL1" s="7" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="GM1" s="7" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="GN1" s="7" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="GO1" s="7" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="GP1" s="7" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="GQ1" s="12" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="GR1" s="12" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="GS1" s="12" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="GT1" s="12" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="GU1" s="12" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="GV1" s="12" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="GW1" s="12" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="GX1" s="12" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="GY1" s="12" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="GZ1" s="12" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="HA1" s="12" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="HB1" s="12" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="HC1" s="12" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="HD1" s="13" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="HE1" s="13" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="HF1" s="13" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="HG1" s="13" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="HH1" s="13" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="HI1" s="13" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="HJ1" s="13" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="HK1" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="HL1" s="13" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="HM1" s="13" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="HN1" s="13" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="HO1" s="13" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="HP1" s="13" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="HQ1" s="14" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="HR1" s="14" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="HS1" s="14" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="HT1" s="14" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="HU1" s="14" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="HV1" s="14" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="HW1" s="14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="HX1" s="14" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="HY1" s="14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="HZ1" s="14" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="IA1" s="14" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="IB1" s="14" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="IC1" s="14" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="ID1" s="15" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="IE1" s="15" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="IF1" s="15" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="IG1" s="15" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="IH1" s="15" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="II1" s="15" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="IJ1" s="15" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="IK1" s="15" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="IL1" s="15" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="IM1" s="15" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="IN1" s="15" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="IO1" s="15" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="IP1" s="15" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="IQ1" s="14" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="IR1" s="14" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="IS1" s="14" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="IT1" s="14" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="IU1" s="14" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="IV1" s="14" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="IW1" s="14" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="IX1" s="14" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="IY1" s="14" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="IZ1" s="14" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="JA1" s="14" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="JB1" s="14" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="JC1" s="14" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="JD1" s="16" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="JE1" s="16" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="JF1" s="16" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="JG1" s="16" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="JH1" s="16" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="JI1" s="16" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="JJ1" s="16" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="JK1" s="16" t="s">
         <v>853</v>
@@ -6015,10 +6015,10 @@
         <v>0</v>
       </c>
       <c r="IM2" s="26" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="IN2" s="26" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="IO2" s="26" t="n">
         <v>10</v>
@@ -7020,13 +7020,13 @@
         <v>82</v>
       </c>
       <c r="FQ3" s="26" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FR3" s="26" t="n">
         <v>0</v>
       </c>
       <c r="FS3" s="26" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="FT3" s="26" t="n">
         <v>61</v>
@@ -7235,13 +7235,13 @@
         <v>0</v>
       </c>
       <c r="IL3" s="26" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="IM3" s="26" t="n">
         <v>0</v>
       </c>
       <c r="IN3" s="26" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="IO3" s="26" t="n">
         <v>65</v>
@@ -8455,7 +8455,7 @@
         <v>32</v>
       </c>
       <c r="IK4" s="26" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="IL4" s="26" t="n">
         <v>15</v>
@@ -8464,7 +8464,7 @@
         <v>55</v>
       </c>
       <c r="IN4" s="26" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="IO4" s="26" t="n">
         <v>21</v>
@@ -9466,13 +9466,13 @@
         <v>74</v>
       </c>
       <c r="FQ5" s="26" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="FR5" s="26" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FS5" s="26" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="FT5" s="26" t="n">
         <v>82</v>
@@ -9678,10 +9678,10 @@
         <v>54</v>
       </c>
       <c r="IK5" s="26" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="IL5" s="26" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="IM5" s="26" t="n">
         <v>89</v>
@@ -10692,7 +10692,7 @@
         <v>84</v>
       </c>
       <c r="FR6" s="26" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="FS6" s="26" t="n">
         <v>83</v>
@@ -10901,7 +10901,7 @@
         <v>87</v>
       </c>
       <c r="IK6" s="26" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="IL6" s="26" t="n">
         <v>99</v>
@@ -11912,13 +11912,13 @@
         <v>52</v>
       </c>
       <c r="FQ7" s="26" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="FR7" s="26" t="n">
         <v>0</v>
       </c>
       <c r="FS7" s="26" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="FT7" s="26" t="n">
         <v>82</v>
@@ -12124,10 +12124,10 @@
         <v>31</v>
       </c>
       <c r="IK7" s="26" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="IL7" s="26" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="IM7" s="26" t="n">
         <v>93</v>
@@ -13347,7 +13347,7 @@
         <v>25</v>
       </c>
       <c r="IK8" s="26" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="IL8" s="26" t="n">
         <v>93</v>
@@ -17016,7 +17016,7 @@
         <v>49</v>
       </c>
       <c r="IK11" s="26" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="IL11" s="26" t="n">
         <v>0</v>
@@ -18347,10 +18347,10 @@
         <v>701</v>
       </c>
       <c r="FQ1" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="FR1" s="11" t="s">
         <v>703</v>
-      </c>
-      <c r="FR1" s="11" t="s">
-        <v>704</v>
       </c>
       <c r="FS1" s="11" t="s">
         <v>705</v>
@@ -18395,250 +18395,250 @@
         <v>723</v>
       </c>
       <c r="GG1" s="7" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="GH1" s="7" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="GI1" s="7" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="GJ1" s="7" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="GK1" s="7" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="GL1" s="7" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="GM1" s="7" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="GN1" s="7" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="GO1" s="7" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="GP1" s="7" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="GQ1" s="12" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="GR1" s="12" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="GS1" s="12" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="GT1" s="12" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="GU1" s="12" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="GV1" s="12" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="GW1" s="12" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="GX1" s="12" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="GY1" s="12" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="GZ1" s="12" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="HA1" s="12" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="HB1" s="12" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="HC1" s="12" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="HD1" s="13" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="HE1" s="13" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="HF1" s="13" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="HG1" s="13" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="HH1" s="13" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="HI1" s="13" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="HJ1" s="13" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="HK1" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="HL1" s="13" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="HM1" s="13" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="HN1" s="13" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="HO1" s="13" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="HP1" s="13" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="HQ1" s="14" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="HR1" s="14" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="HS1" s="14" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="HT1" s="14" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="HU1" s="14" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="HV1" s="14" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="HW1" s="14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="HX1" s="14" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="HY1" s="14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="HZ1" s="14" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="IA1" s="14" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="IB1" s="14" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="IC1" s="14" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="ID1" s="15" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="IE1" s="15" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="IF1" s="15" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="IG1" s="15" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="IH1" s="15" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="II1" s="15" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="IJ1" s="15" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="IK1" s="15" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="IL1" s="15" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="IM1" s="15" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="IN1" s="15" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="IO1" s="15" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="IP1" s="15" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="IQ1" s="14" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="IR1" s="14" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="IS1" s="14" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="IT1" s="14" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="IU1" s="14" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="IV1" s="14" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="IW1" s="14" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="IX1" s="14" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="IY1" s="14" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="IZ1" s="14" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="JA1" s="14" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="JB1" s="14" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="JC1" s="14" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="JD1" s="16" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="JE1" s="16" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="JF1" s="16" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="JG1" s="16" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="JH1" s="16" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="JI1" s="16" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="JJ1" s="16" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="JK1" s="16" t="s">
         <v>853</v>
@@ -19564,13 +19564,13 @@
         <v>57.6216050626212</v>
       </c>
       <c r="FQ2" s="26" t="n">
-        <v>26.0844119852241</v>
+        <v>84.9423601169581</v>
       </c>
       <c r="FR2" s="26" t="n">
-        <v>5.02618445096331</v>
+        <v>37.931634588221</v>
       </c>
       <c r="FS2" s="26" t="n">
-        <v>26.3473274981435</v>
+        <v>85.612347469941</v>
       </c>
       <c r="FT2" s="26" t="n">
         <v>68.8657580521925</v>
@@ -19776,16 +19776,16 @@
         <v>46.4249874543021</v>
       </c>
       <c r="IK2" s="26" t="n">
-        <v>3.76963833822248</v>
+        <v>69.7121730817598</v>
       </c>
       <c r="IL2" s="26" t="n">
-        <v>26.6169908681623</v>
+        <v>82.3314591272486</v>
       </c>
       <c r="IM2" s="26" t="n">
-        <v>78.9323777941743</v>
+        <v>79.1870584420925</v>
       </c>
       <c r="IN2" s="26" t="n">
-        <v>43.5815947161454</v>
+        <v>47.1976415279885</v>
       </c>
       <c r="IO2" s="26" t="n">
         <v>60.1564576670604</v>
@@ -21806,23 +21806,23 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>647</v>
+      </c>
+      <c r="B174" t="s">
         <v>702</v>
-      </c>
-      <c r="B174" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>567</v>
+        <v>656</v>
       </c>
       <c r="B175" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B176" t="s">
         <v>705</v>
@@ -21934,10 +21934,10 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>702</v>
+        <v>724</v>
       </c>
       <c r="B190" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="191">
@@ -21945,7 +21945,7 @@
         <v>562</v>
       </c>
       <c r="B191" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="192">
@@ -21953,7 +21953,7 @@
         <v>3</v>
       </c>
       <c r="B192" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="193">
@@ -21961,7 +21961,7 @@
         <v>496</v>
       </c>
       <c r="B193" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="194">
@@ -21969,7 +21969,7 @@
         <v>496</v>
       </c>
       <c r="B194" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="195">
@@ -21977,7 +21977,7 @@
         <v>7</v>
       </c>
       <c r="B195" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="196">
@@ -21985,7 +21985,7 @@
         <v>678</v>
       </c>
       <c r="B196" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="197">
@@ -21993,15 +21993,15 @@
         <v>620</v>
       </c>
       <c r="B197" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B198" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="199">
@@ -22009,71 +22009,71 @@
         <v>612</v>
       </c>
       <c r="B199" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B200" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B201" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B202" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B203" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B204" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B205" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B206" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B207" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="208">
@@ -22081,37 +22081,37 @@
         <v>505</v>
       </c>
       <c r="B208" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B209" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B210" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B211" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="212">
       <c r="A212"/>
       <c r="B212" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="213">
@@ -22119,31 +22119,31 @@
         <v>633</v>
       </c>
       <c r="B213" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B214" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B215" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B216" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="217">
@@ -22151,7 +22151,7 @@
         <v>628</v>
       </c>
       <c r="B217" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="218">
@@ -22159,15 +22159,15 @@
         <v>633</v>
       </c>
       <c r="B218" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B219" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="220">
@@ -22175,7 +22175,7 @@
         <v>651</v>
       </c>
       <c r="B220" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="221">
@@ -22183,7 +22183,7 @@
         <v>651</v>
       </c>
       <c r="B221" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="222">
@@ -22191,15 +22191,15 @@
         <v>649</v>
       </c>
       <c r="B222" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B223" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="224">
@@ -22207,61 +22207,61 @@
         <v>623</v>
       </c>
       <c r="B224" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="225">
       <c r="A225"/>
       <c r="B225" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B226" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B227" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B228" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B229" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B230" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B231" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="232">
@@ -22269,23 +22269,23 @@
         <v>517</v>
       </c>
       <c r="B232" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B233" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B234" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="235">
@@ -22293,23 +22293,23 @@
         <v>490</v>
       </c>
       <c r="B235" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B236" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B237" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="238">
@@ -22317,7 +22317,7 @@
         <v>481</v>
       </c>
       <c r="B238" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="239">
@@ -22325,15 +22325,15 @@
         <v>628</v>
       </c>
       <c r="B239" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B240" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="241">
@@ -22341,15 +22341,15 @@
         <v>616</v>
       </c>
       <c r="B241" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B242" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="243">
@@ -22357,7 +22357,7 @@
         <v>616</v>
       </c>
       <c r="B243" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="244">
@@ -22365,47 +22365,47 @@
         <v>628</v>
       </c>
       <c r="B244" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B245" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>488</v>
+        <v>628</v>
       </c>
       <c r="B246" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>578</v>
+        <v>811</v>
       </c>
       <c r="B247" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B248" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B249" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row r="250">
@@ -22413,117 +22413,117 @@
         <v>680</v>
       </c>
       <c r="B250" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="251">
       <c r="A251"/>
       <c r="B251" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B252" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B253" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="B254" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B255" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B256" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B257" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B258" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="B259" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B260" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B261" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B262" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B263" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B264" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="265">
@@ -22531,7 +22531,7 @@
         <v>623</v>
       </c>
       <c r="B265" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
     <row r="266">
@@ -22539,7 +22539,7 @@
         <v>642</v>
       </c>
       <c r="B266" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="267">
@@ -22547,7 +22547,7 @@
         <v>645</v>
       </c>
       <c r="B267" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="268">
@@ -22555,36 +22555,36 @@
         <v>647</v>
       </c>
       <c r="B268" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B269" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>848</v>
+        <v>811</v>
       </c>
       <c r="B270" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B271" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>852</v>
+        <v>704</v>
       </c>
       <c r="B272" t="s">
         <v>853</v>
@@ -22608,7 +22608,7 @@
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B275" t="s">
         <v>856</v>
@@ -22640,7 +22640,7 @@
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B279" t="s">
         <v>861</v>
@@ -22688,7 +22688,7 @@
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>852</v>
+        <v>704</v>
       </c>
       <c r="B285" t="s">
         <v>870</v>
@@ -22696,7 +22696,7 @@
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>848</v>
+        <v>811</v>
       </c>
       <c r="B286" t="s">
         <v>871</v>
@@ -22704,7 +22704,7 @@
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>852</v>
+        <v>704</v>
       </c>
       <c r="B287" t="s">
         <v>872</v>
@@ -23032,7 +23032,7 @@
     </row>
     <row r="328">
       <c r="A328" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B328" t="s">
         <v>928</v>

</xml_diff>